<commit_message>
new code testng - dataprovider
</commit_message>
<xml_diff>
--- a/src/test/resources/configproperties/TestData_Swaglab_Data.xlsx
+++ b/src/test/resources/configproperties/TestData_Swaglab_Data.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29520" windowHeight="11360"/>
+    <workbookView windowHeight="13760"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Username</t>
   </si>
@@ -35,9 +36,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Keyword</t>
-  </si>
-  <si>
     <t>Result</t>
   </si>
   <si>
@@ -53,10 +51,34 @@
     <t>problem_user</t>
   </si>
   <si>
+    <t>0,0</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t>0,2</t>
+  </si>
+  <si>
+    <t>0,3</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>1,4</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -1007,19 +1029,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.6" outlineLevelRow="3" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.6" outlineLevelRow="3" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.8308823529412"/>
-    <col min="2" max="2" customWidth="true" width="13.5"/>
+    <col min="1" max="1" width="13.8308823529412" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1029,45 +1051,106 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s" s="0">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s" s="0">
-        <v>9</v>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>8</v>
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.94117647058824" defaultRowHeight="17.6" outlineLevelRow="3" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="14.8823529411765" customWidth="1"/>
+    <col min="2" max="2" width="12.0588235294118" customWidth="1"/>
+    <col min="3" max="3" width="8.88235294117647" customWidth="1"/>
+    <col min="4" max="4" width="6.82352941176471" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
data providers updated files
</commit_message>
<xml_diff>
--- a/src/test/resources/configproperties/TestData_Swaglab_Data.xlsx
+++ b/src/test/resources/configproperties/TestData_Swaglab_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11300"/>
+    <workbookView windowWidth="28800" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -1007,7 +1007,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.6" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -1046,7 +1046,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>